<commit_message>
[Task 4] v2 Import excel file with street factors and improvements
	- Create a template xlsx with column names of factors and street names as sheet names.
	- Create a factors data in xlsx.
	- Save import data from excel file into DB.
	- Improve code structure.
	- Segregate experimental codes.
</commit_message>
<xml_diff>
--- a/curves.xlsx
+++ b/curves.xlsx
@@ -12,8 +12,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7680"/>
   </bookViews>
   <sheets>
-    <sheet name="edges sheet" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="curves sheet" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t>curve id</t>
   </si>
@@ -184,153 +183,6 @@
   </si>
   <si>
     <t>10.325932,123.907650:10.326202,123.907905:10.331775,123.910276:10.333147,123.910523:10.339005,123.911585:10.339945,123.911832:10.349032,123.913334:10.350489,123.913549:10.351481,123.913817:10.352452,123.913988:10.354911,123.914739:10.355734,123.915094:10.357792,123.915169:10.358626,123.915705:10.360948,123.91534:10.362204,123.91534:10.364388,123.914654:10.36538,123.913838:10.367523,123.913913:10.371569:123.923957</t>
-  </si>
-  <si>
-    <t>10_11:10.307819,123.886707:10.305099,123.886696:10.303706,123.886846:10.300539,123.886718:10.297221,123.888381</t>
-  </si>
-  <si>
-    <t>9_10:10.315672,123.885634:10.312952,123.886160:10.312404,123.886138:10.310250,123.886482:10.307819,123.886707</t>
-  </si>
-  <si>
-    <t>4_2:10.289747,123.870742:10.290338,123.876278</t>
-  </si>
-  <si>
-    <t>1_2:10.271590,123.847311:10.279418,123.855304:10.282817,123.858286:10.286976,123.862127:10.288834,123.866633:10.289747,123.870742</t>
-  </si>
-  <si>
-    <t>30_4:10.270092,123.856403:10.270419,123.856779,10.274620,123.859912:10.274737,123.860115:10.283119,123.866714:10.284808,123.868516:10.290338,123.876278</t>
-  </si>
-  <si>
-    <t>2_3:10.289747,123.870742:10.292429,123.870533:10.293685,123.870329:10.295469,123.869868:10.297243,123.869889:10.298372,123.869825:10.299639,123.869932:10.300959,123.869686:10.301443,123.870442</t>
-  </si>
-  <si>
-    <t>4_7:10.290338,123.876278:10.296134,123.884395:10.296858,123.886136:10.297136,123.887994</t>
-  </si>
-  <si>
-    <t>4_5:10.290338,123.876278:10.290634,123.877695</t>
-  </si>
-  <si>
-    <t>3_6:10.301443,123.870442:10.299543,123.878982</t>
-  </si>
-  <si>
-    <t>6_7:10.299543,123.878982:10.297136,123.887994</t>
-  </si>
-  <si>
-    <t>7_11:10.297136,123.887994:10.297221,123.888381</t>
-  </si>
-  <si>
-    <t>6_9:10.299543,123.878982:10.302737,123.877949:10.305207,123.876532:10.306157,123.876168:10.307339,123.875974:10.309873,123.876082:10.312469,123.877991:10.313630,123.880030:10.314665,123.882540:10.315672,123.885634</t>
-  </si>
-  <si>
-    <t>8_9:10.315672,123.885634:10.323510,123.883721:10.324186,123.883356:10.324861,123.883227:10.329267,123.881085</t>
-  </si>
-  <si>
-    <t>11_12:10.297221,123.888381:10.297660,123.890921:10.298315,123.892499:10.298705,123.895224:10.299459,123.896921</t>
-  </si>
-  <si>
-    <t>12_13:10.299459,123.896921:10.297723,123.897530:10.296225,123.898239</t>
-  </si>
-  <si>
-    <t>5_13:10.290634,123.877695:10.290883,123.878455:10.292920,123.885900:10.293860,123.890964:10.294251,123.893518:10.296165,123.898294</t>
-  </si>
-  <si>
-    <t>9_20:10.315672,123.885634:10.316238,123.886909:10.317199,123.889838:10.316027,123.890235:10.316094,123.890955</t>
-  </si>
-  <si>
-    <t>10_17:10.307819,123.886707:10.307942,123.887156:10.308121,123.889398:10.309339,123.892629</t>
-  </si>
-  <si>
-    <t>20_18:10.316094,123.890955:10.310479,123.892887</t>
-  </si>
-  <si>
-    <t>28_17:10.310479,123.892887:10.310179,123.892563:10.309715,123.892456:10.309339,123.892629</t>
-  </si>
-  <si>
-    <t>17_16:10.309339,123.892629:10.309086,123.893445</t>
-  </si>
-  <si>
-    <t>18_19:10.310479,123.892887:10.310475,123.893432:10.310232,123.893722:10.309803,123.893917</t>
-  </si>
-  <si>
-    <t>19_16:10.309803,123.893917:10.309086,123.893445</t>
-  </si>
-  <si>
-    <t>12_16:10.299459,123.896921:10.309086,123.893445</t>
-  </si>
-  <si>
-    <t>13_15:10.296165,123.898294:10.293563,123.904592:10.294419,123.905094</t>
-  </si>
-  <si>
-    <t>15_14:10.294419,123.905094:10.293970,123.906062</t>
-  </si>
-  <si>
-    <t>12_24:10.299459,123.896921:10.301418,123.900320:10.302073,123.902133:10.302358,123.902444:10.308790,123.907135</t>
-  </si>
-  <si>
-    <t>15_24:10.294419,123.905094:10.295623,123.905502:10.29727,123.905888:10.301313,123.906586:10.302315,123.906532:10.305018,123.906167:10.306358,123.906124:10.307393,123.906457:10.307994,123.906779:10.308438,123.90694:10.308790,123.907135</t>
-  </si>
-  <si>
-    <t>20_21:10.316094,123.890955:10.317494,123.894623:10.318459,123.900011</t>
-  </si>
-  <si>
-    <t>21_34:10.318459,123.900011:10.319933,123.899344:10.322413,123.898764:10.325326,123.898142:10.326941,123.897927:10.328641,123.897423:10.331131,123.898099:10.330998,123.898165</t>
-  </si>
-  <si>
-    <t>21_22:10.318459,123.900011:10.31761,123.900459:10.315461,123.901684</t>
-  </si>
-  <si>
-    <t>21_31:10.318459,123.900011:10.320429,123.903689:10.320317,123.903873</t>
-  </si>
-  <si>
-    <t>22_31:10.315461,123.901684:10.317737,123.902627:10.318645,123.903056:10.320317,123.903873</t>
-  </si>
-  <si>
-    <t>22_23:10.315461,123.901684:10.313156,123.902755:10.310732,123.903873</t>
-  </si>
-  <si>
-    <t>19_23:10.309803,123.893917:10.311193,123.898206:10.311478,123.89958:10.311267,123.902444:10.310732,123.903873</t>
-  </si>
-  <si>
-    <t>23_24:10.310732,123.903873:10.308790,123.907135</t>
-  </si>
-  <si>
-    <t>24_25:10.308790,123.907135:10.307101,123.909924</t>
-  </si>
-  <si>
-    <t>25_26:10.307101,123.909924:10.303597,123.912756</t>
-  </si>
-  <si>
-    <t>26_27:10.303597,123.912756:10.308832,123.919151</t>
-  </si>
-  <si>
-    <t>27_28:10.308832,123.919151:10.312294,123.916233</t>
-  </si>
-  <si>
-    <t>28_25:10.312294,123.916233:10.307101,123.909924</t>
-  </si>
-  <si>
-    <t>28_29:10.312294,123.916233:10.313768,123.914986:10.314194,123.914688</t>
-  </si>
-  <si>
-    <t>29_24:10.314194,123.914688:10.311953,123.909944:10.310538,123.90857:10.308790,123.907135</t>
-  </si>
-  <si>
-    <t>31_30:10.320317,123.903873:10.325932,123.907650</t>
-  </si>
-  <si>
-    <t>34_30:10.330998,123.898165:10.3271,123.906081:10.325932,123.907650</t>
-  </si>
-  <si>
-    <t>29_30:10.314194,123.914688:10.325932,123.907650</t>
-  </si>
-  <si>
-    <t>14_26:10.293970,123.906062:10.293976,123.906028:10.301513,123.910201:10.303597,123.912756</t>
-  </si>
-  <si>
-    <t>14_5:10.293970,123.906062:10.291569,123.90371:10.291231,123.903442:10.290197,123.899376:10.288677,123.897766:10.287917,123.889645:10.2819,123.883529:10.284919,123.880407:10.286798,123.879828:10.289342,123.87854:10.290634,123.877695</t>
-  </si>
-  <si>
-    <t>30_32:10.325932,123.907650:10.326202,123.907905:10.331775,123.910276:10.333147,123.910523:10.339005,123.911585:10.339945,123.911832:10.349032,123.913334:10.350489,123.913549:10.351481,123.913817:10.352452,123.913988:10.354911,123.914739:10.355734,123.915094:10.357792,123.915169:10.358626,123.915705:10.360948,123.91534:10.362204,123.91534:10.364388,123.914654:10.36538,123.913838:10.367523,123.913913:10.371569:123.923957</t>
   </si>
 </sst>
 </file>
@@ -685,7 +537,7 @@
   <dimension ref="A1:D50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
+      <selection activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1393,264 +1245,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A49"/>
-  <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection sqref="A1:A49"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>101</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>